<commit_message>
Backup before nectec version ,Remove speaker, Add Light (LDR) an d FanDC
</commit_message>
<xml_diff>
--- a/newscript/MakerPlaygroundActualDeviceListCheck.xlsx
+++ b/newscript/MakerPlaygroundActualDeviceListCheck.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
   <si>
     <t>รายการสินค้า</t>
   </si>
@@ -728,12 +728,33 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Adafruit LSM303</t>
+  </si>
+  <si>
+    <t>Infrared Barrier tracking avoidance Obstacle Sensor Module โมดูลตรวจจับเส้นและสิ่งกีดขวางแบบอินฟาเรด</t>
+  </si>
+  <si>
+    <t>Light Dependent Resistor LDR 5MM Photoresistor</t>
+  </si>
+  <si>
+    <t>Module MQ-2 FC-22 Smoke Gas Sensor Smoke methane gas liquefied flammable gas sensor module for arduano</t>
+  </si>
+  <si>
+    <t>Soil Moisture Sensor Module</t>
+  </si>
+  <si>
+    <t>โมดูล เซนเซอร์น้ำฝน / ระดับน้ำ Rain Raindrop Water Level Sensor Module Height Depth of Detection For Arduino</t>
+  </si>
+  <si>
+    <t>Fan dC Motor Module L9110 Fan Module for Arduino</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,6 +824,26 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -904,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -924,23 +965,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -960,6 +989,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,17 +1015,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2991,13 +3046,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>609600</xdr:rowOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3021,8 +3076,338 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="80727550"/>
-          <a:ext cx="609600" cy="609600"/>
+          <a:off x="0" y="26060400"/>
+          <a:ext cx="609600" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>482600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43" descr="Infrared Barrier tracking avoidance Obstacle Sensor Module โมดูลตรวจจับเส้นและสิ่งกีดขวางแบบอินฟาเรด"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6350" y="31172150"/>
+          <a:ext cx="565150" cy="565150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>35386</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>469900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44" descr="Light Dependent Resistor LDR 5MM Photoresistor"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="31826200"/>
+          <a:ext cx="644986" cy="349250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45" descr="Module MQ-2 FC-22 Smoke Gas Sensor Smoke methane gas liquefied flammable gas sensor module for arduano"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="32213550"/>
+          <a:ext cx="508000" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46" descr="Soil Moisture Sensor Module"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="32721550"/>
+          <a:ext cx="546100" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47" descr="โมดูล เซนเซอร์น้ำฝน / ระดับน้ำ Rain Raindrop Water Level Sensor Module Height Depth of Detection For Arduino"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="33229550"/>
+          <a:ext cx="533400" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48" descr="Fan dC Motor Module L9110 Fan Module for Arduino"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="33737550"/>
+          <a:ext cx="527050" cy="527050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3307,10 +3692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3321,12 +3706,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="8" t="s">
         <v>85</v>
       </c>
@@ -3344,14 +3729,14 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>88</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -3371,14 +3756,14 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="29">
         <v>2</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="29">
         <v>550</v>
       </c>
       <c r="E3" s="2"/>
@@ -3388,12 +3773,12 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="3"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3401,14 +3786,14 @@
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="29">
         <v>105</v>
       </c>
       <c r="E5" s="2"/>
@@ -3418,12 +3803,12 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="3"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -3431,14 +3816,14 @@
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="29">
         <v>1</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="29">
         <v>60</v>
       </c>
       <c r="E7" s="2"/>
@@ -3448,12 +3833,12 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="3"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -3461,14 +3846,14 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="29">
         <v>120</v>
       </c>
       <c r="E9" s="2"/>
@@ -3478,12 +3863,12 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="3"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -3491,14 +3876,14 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="29">
         <v>1</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="29">
         <v>75</v>
       </c>
       <c r="E11" s="2"/>
@@ -3508,12 +3893,12 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="3"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -3521,14 +3906,14 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="29">
         <v>1</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="29">
         <v>380</v>
       </c>
       <c r="E13" s="2"/>
@@ -3538,12 +3923,12 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="3"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -3551,14 +3936,14 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="29">
         <v>1</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="29">
         <v>190</v>
       </c>
       <c r="E15" s="2"/>
@@ -3568,12 +3953,12 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="3"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -3581,14 +3966,14 @@
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="31"/>
+      <c r="B17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="29">
         <v>1</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="29">
         <v>95</v>
       </c>
       <c r="E17" s="2"/>
@@ -3598,12 +3983,12 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="3"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -3611,14 +3996,14 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="29">
         <v>1</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="29">
         <v>85</v>
       </c>
       <c r="E19" s="2"/>
@@ -3628,12 +4013,12 @@
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="31"/>
+      <c r="B20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="3"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -3641,14 +4026,14 @@
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="29">
         <v>1</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="29">
         <v>125</v>
       </c>
       <c r="E21" s="2"/>
@@ -3658,12 +4043,12 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="3"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -3671,14 +4056,14 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="31"/>
+      <c r="B23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="29">
         <v>1</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="29">
         <v>300</v>
       </c>
       <c r="E23" s="2"/>
@@ -3688,12 +4073,12 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="3"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -3701,14 +4086,14 @@
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="29">
         <v>1</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="29">
         <v>90</v>
       </c>
       <c r="E25" s="2"/>
@@ -3718,12 +4103,12 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="3"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -3731,23 +4116,23 @@
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="8" t="s">
         <v>85</v>
       </c>
@@ -3765,14 +4150,14 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="11" t="s">
         <v>88</v>
       </c>
       <c r="E29" s="9" t="s">
@@ -3792,14 +4177,14 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="31"/>
+      <c r="B30" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="29">
         <v>1</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="29">
         <v>175</v>
       </c>
       <c r="E30" s="2"/>
@@ -3809,12 +4194,12 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="31"/>
+      <c r="B31" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="3"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -3822,14 +4207,14 @@
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="29">
         <v>1</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="29">
         <v>200</v>
       </c>
       <c r="E32" s="2"/>
@@ -3839,12 +4224,12 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="3"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -3852,14 +4237,14 @@
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15" t="s">
+      <c r="A34" s="31"/>
+      <c r="B34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="29">
         <v>1</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="29">
         <v>65</v>
       </c>
       <c r="E34" s="2"/>
@@ -3869,12 +4254,12 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="3"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -3882,14 +4267,14 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="29">
         <v>1</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="29">
         <v>120</v>
       </c>
       <c r="E36" s="2"/>
@@ -3899,12 +4284,12 @@
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="31"/>
+      <c r="B37" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
       <c r="E37" s="3"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -3912,14 +4297,14 @@
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="29">
         <v>1</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="29">
         <v>120</v>
       </c>
       <c r="E38" s="2"/>
@@ -3929,12 +4314,12 @@
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
-      <c r="B39" s="17" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
       <c r="E39" s="3"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -3942,14 +4327,14 @@
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="31"/>
+      <c r="B40" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="29">
         <v>1</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="29">
         <v>60</v>
       </c>
       <c r="E40" s="2"/>
@@ -3959,12 +4344,12 @@
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17" t="s">
+      <c r="A41" s="31"/>
+      <c r="B41" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="3"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -3972,14 +4357,14 @@
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="31"/>
+      <c r="B42" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="29">
         <v>1</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="29">
         <v>145</v>
       </c>
       <c r="E42" s="2"/>
@@ -3989,12 +4374,12 @@
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="3"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -4002,29 +4387,33 @@
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="29">
         <v>1</v>
       </c>
-      <c r="D44" s="16">
+      <c r="D44" s="29">
         <v>70</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="5"/>
+      <c r="E44" s="33">
+        <v>43017</v>
+      </c>
+      <c r="F44" s="33">
+        <v>43017</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="31"/>
+      <c r="B45" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
       <c r="E45" s="3"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -4032,14 +4421,14 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="16">
+      <c r="C46" s="29">
         <v>1</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="29">
         <v>170</v>
       </c>
       <c r="E46" s="2"/>
@@ -4049,12 +4438,12 @@
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
       <c r="E47" s="3"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -4062,14 +4451,14 @@
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="29">
         <v>1</v>
       </c>
-      <c r="D48" s="16">
+      <c r="D48" s="29">
         <v>20</v>
       </c>
       <c r="E48" s="2"/>
@@ -4079,12 +4468,12 @@
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
       <c r="E49" s="3"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -4092,14 +4481,14 @@
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="14"/>
-      <c r="B50" s="15" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="29">
         <v>1</v>
       </c>
-      <c r="D50" s="16">
+      <c r="D50" s="29">
         <v>110</v>
       </c>
       <c r="E50" s="2"/>
@@ -4109,12 +4498,12 @@
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17" t="s">
+      <c r="A51" s="31"/>
+      <c r="B51" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
       <c r="E51" s="3"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -4122,14 +4511,14 @@
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14"/>
-      <c r="B52" s="15" t="s">
+      <c r="A52" s="31"/>
+      <c r="B52" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52" s="29">
         <v>1</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="29">
         <v>235</v>
       </c>
       <c r="E52" s="2"/>
@@ -4139,32 +4528,32 @@
       <c r="I52" s="5"/>
     </row>
     <row r="53" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="14"/>
-      <c r="B53" s="17" t="s">
+      <c r="A53" s="31"/>
+      <c r="B53" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
       <c r="E53" s="3"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="28"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="31"/>
+    <row r="54" spans="1:9" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="22"/>
     </row>
     <row r="55" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28"/>
       <c r="E55" s="8" t="s">
         <v>85</v>
       </c>
@@ -4182,14 +4571,14 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="13" t="s">
+      <c r="B56" s="25"/>
+      <c r="C56" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" s="11" t="s">
         <v>88</v>
       </c>
       <c r="E56" s="9" t="s">
@@ -4209,14 +4598,14 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="14"/>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="31"/>
+      <c r="B57" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C57" s="29">
         <v>1</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="29">
         <v>225</v>
       </c>
       <c r="E57" s="2"/>
@@ -4226,12 +4615,12 @@
       <c r="I57" s="5"/>
     </row>
     <row r="58" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17" t="s">
+      <c r="A58" s="31"/>
+      <c r="B58" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
       <c r="E58" s="3"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -4239,29 +4628,33 @@
       <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="14"/>
-      <c r="B59" s="15" t="s">
+      <c r="A59" s="31"/>
+      <c r="B59" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C59" s="29">
         <v>1</v>
       </c>
-      <c r="D59" s="16">
+      <c r="D59" s="29">
         <v>40</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="5"/>
+      <c r="E59" s="33">
+        <v>42988</v>
+      </c>
+      <c r="F59" s="33">
+        <v>42988</v>
+      </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="14"/>
-      <c r="B60" s="17" t="s">
+      <c r="A60" s="31"/>
+      <c r="B60" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
       <c r="E60" s="3"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -4269,14 +4662,14 @@
       <c r="I60" s="6"/>
     </row>
     <row r="61" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="14"/>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="31"/>
+      <c r="B61" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C61" s="16">
+      <c r="C61" s="29">
         <v>1</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D61" s="29">
         <v>75</v>
       </c>
       <c r="E61" s="2"/>
@@ -4286,12 +4679,12 @@
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="14"/>
-      <c r="B62" s="17" t="s">
+      <c r="A62" s="31"/>
+      <c r="B62" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
       <c r="E62" s="3"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -4299,14 +4692,14 @@
       <c r="I62" s="6"/>
     </row>
     <row r="63" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="14"/>
-      <c r="B63" s="15" t="s">
+      <c r="A63" s="31"/>
+      <c r="B63" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C63" s="16">
+      <c r="C63" s="29">
         <v>1</v>
       </c>
-      <c r="D63" s="16">
+      <c r="D63" s="29">
         <v>120</v>
       </c>
       <c r="E63" s="2"/>
@@ -4316,12 +4709,12 @@
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17" t="s">
+      <c r="A64" s="31"/>
+      <c r="B64" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
       <c r="E64" s="3"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
@@ -4329,14 +4722,14 @@
       <c r="I64" s="6"/>
     </row>
     <row r="65" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="14"/>
-      <c r="B65" s="15" t="s">
+      <c r="A65" s="31"/>
+      <c r="B65" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="16">
+      <c r="C65" s="29">
         <v>1</v>
       </c>
-      <c r="D65" s="16">
+      <c r="D65" s="29">
         <v>95</v>
       </c>
       <c r="E65" s="2"/>
@@ -4346,12 +4739,12 @@
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17" t="s">
+      <c r="A66" s="31"/>
+      <c r="B66" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
       <c r="E66" s="3"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
@@ -4359,14 +4752,14 @@
       <c r="I66" s="6"/>
     </row>
     <row r="67" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="14"/>
-      <c r="B67" s="15" t="s">
+      <c r="A67" s="31"/>
+      <c r="B67" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="16">
+      <c r="C67" s="29">
         <v>1</v>
       </c>
-      <c r="D67" s="16">
+      <c r="D67" s="29">
         <v>95</v>
       </c>
       <c r="E67" s="2"/>
@@ -4376,12 +4769,12 @@
       <c r="I67" s="5"/>
     </row>
     <row r="68" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="14"/>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="31"/>
+      <c r="B68" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
       <c r="E68" s="3"/>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -4389,14 +4782,14 @@
       <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="14"/>
-      <c r="B69" s="15" t="s">
+      <c r="A69" s="31"/>
+      <c r="B69" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C69" s="16">
+      <c r="C69" s="29">
         <v>1</v>
       </c>
-      <c r="D69" s="16">
+      <c r="D69" s="29">
         <v>85</v>
       </c>
       <c r="E69" s="2"/>
@@ -4406,12 +4799,12 @@
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17" t="s">
+      <c r="A70" s="31"/>
+      <c r="B70" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
       <c r="E70" s="3"/>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
@@ -4419,29 +4812,33 @@
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="14"/>
-      <c r="B71" s="15" t="s">
+      <c r="A71" s="31"/>
+      <c r="B71" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C71" s="16">
+      <c r="C71" s="29">
         <v>1</v>
       </c>
-      <c r="D71" s="16">
+      <c r="D71" s="29">
         <v>100</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="5"/>
+      <c r="E71" s="33">
+        <v>42988</v>
+      </c>
+      <c r="F71" s="33">
+        <v>42988</v>
+      </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17" t="s">
+      <c r="A72" s="31"/>
+      <c r="B72" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
       <c r="E72" s="3"/>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -4449,14 +4846,14 @@
       <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="14"/>
-      <c r="B73" s="15" t="s">
+      <c r="A73" s="31"/>
+      <c r="B73" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="16">
+      <c r="C73" s="29">
         <v>1</v>
       </c>
-      <c r="D73" s="16">
+      <c r="D73" s="29">
         <v>200</v>
       </c>
       <c r="E73" s="2"/>
@@ -4466,12 +4863,12 @@
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="14"/>
-      <c r="B74" s="17" t="s">
+      <c r="A74" s="31"/>
+      <c r="B74" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
       <c r="E74" s="3"/>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
@@ -4479,29 +4876,33 @@
       <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="14"/>
-      <c r="B75" s="15" t="s">
+      <c r="A75" s="31"/>
+      <c r="B75" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C75" s="16">
+      <c r="C75" s="29">
         <v>1</v>
       </c>
-      <c r="D75" s="16">
+      <c r="D75" s="29">
         <v>75</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="5"/>
+      <c r="E75" s="33">
+        <v>42988</v>
+      </c>
+      <c r="F75" s="33">
+        <v>42988</v>
+      </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="14"/>
-      <c r="B76" s="17" t="s">
+      <c r="A76" s="31"/>
+      <c r="B76" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
       <c r="E76" s="3"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
@@ -4509,14 +4910,14 @@
       <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="14"/>
-      <c r="B77" s="15" t="s">
+      <c r="A77" s="31"/>
+      <c r="B77" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C77" s="16">
+      <c r="C77" s="29">
         <v>1</v>
       </c>
-      <c r="D77" s="16">
+      <c r="D77" s="29">
         <v>70</v>
       </c>
       <c r="E77" s="2"/>
@@ -4526,12 +4927,12 @@
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17" t="s">
+      <c r="A78" s="31"/>
+      <c r="B78" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
       <c r="E78" s="3"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
@@ -4539,14 +4940,14 @@
       <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="14"/>
-      <c r="B79" s="15" t="s">
+      <c r="A79" s="31"/>
+      <c r="B79" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C79" s="16">
+      <c r="C79" s="29">
         <v>1</v>
       </c>
-      <c r="D79" s="16">
+      <c r="D79" s="29">
         <v>300</v>
       </c>
       <c r="E79" s="2"/>
@@ -4556,32 +4957,32 @@
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17" t="s">
+      <c r="A80" s="31"/>
+      <c r="B80" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
       <c r="E80" s="3"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="1:9" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="28"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="31"/>
+    <row r="81" spans="1:9" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="19"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="22"/>
     </row>
     <row r="82" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="25" t="s">
+      <c r="A82" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="26"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="28"/>
       <c r="E82" s="8" t="s">
         <v>85</v>
       </c>
@@ -4599,14 +5000,14 @@
       </c>
     </row>
     <row r="83" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="24"/>
-      <c r="C83" s="13" t="s">
+      <c r="B83" s="25"/>
+      <c r="C83" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="11" t="s">
         <v>88</v>
       </c>
       <c r="E83" s="9" t="s">
@@ -4626,14 +5027,14 @@
       </c>
     </row>
     <row r="84" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="14"/>
-      <c r="B84" s="15" t="s">
+      <c r="A84" s="31"/>
+      <c r="B84" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C84" s="16">
+      <c r="C84" s="29">
         <v>1</v>
       </c>
-      <c r="D84" s="16">
+      <c r="D84" s="29">
         <v>70</v>
       </c>
       <c r="E84" s="2"/>
@@ -4643,12 +5044,12 @@
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="14"/>
-      <c r="B85" s="17" t="s">
+      <c r="A85" s="31"/>
+      <c r="B85" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
       <c r="E85" s="3"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
@@ -4656,16 +5057,16 @@
       <c r="I85" s="6"/>
     </row>
     <row r="86" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C86" s="19">
+      <c r="C86" s="15">
         <v>1</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="15" t="s">
         <v>89</v>
       </c>
       <c r="E86" s="4"/>
@@ -4675,35 +5076,39 @@
       <c r="I86" s="7"/>
     </row>
     <row r="87" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="22" t="s">
+      <c r="A87" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C87" s="20">
+      <c r="C87" s="16">
         <v>1</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="4"/>
-      <c r="F87" s="7"/>
+      <c r="E87" s="34">
+        <v>42986</v>
+      </c>
+      <c r="F87" s="34">
+        <v>42986</v>
+      </c>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
     </row>
     <row r="88" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="22" t="s">
+      <c r="A88" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C88" s="20">
+      <c r="C88" s="16">
         <v>1</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D88" s="15" t="s">
         <v>89</v>
       </c>
       <c r="E88" s="4"/>
@@ -4713,92 +5118,108 @@
       <c r="I88" s="7"/>
     </row>
     <row r="89" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C89" s="20">
+      <c r="C89" s="16">
         <v>1</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E89" s="4"/>
-      <c r="F89" s="7"/>
+      <c r="E89" s="34">
+        <v>42986</v>
+      </c>
+      <c r="F89" s="34">
+        <v>42986</v>
+      </c>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
     </row>
     <row r="90" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="22" t="s">
+      <c r="A90" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="18" t="s">
+      <c r="B90" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C90" s="20">
+      <c r="C90" s="16">
         <v>1</v>
       </c>
-      <c r="D90" s="19" t="s">
+      <c r="D90" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E90" s="4"/>
-      <c r="F90" s="7"/>
+      <c r="E90" s="34">
+        <v>42986</v>
+      </c>
+      <c r="F90" s="34">
+        <v>42986</v>
+      </c>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
     </row>
     <row r="91" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="22" t="s">
+      <c r="A91" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="20">
+      <c r="C91" s="16">
         <v>1</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E91" s="4"/>
-      <c r="F91" s="7"/>
+      <c r="E91" s="34">
+        <v>42986</v>
+      </c>
+      <c r="F91" s="34">
+        <v>42986</v>
+      </c>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
     </row>
     <row r="92" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="22" t="s">
+      <c r="A92" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B92" s="18" t="s">
+      <c r="B92" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C92" s="20">
+      <c r="C92" s="16">
         <v>1</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="7"/>
+      <c r="E92" s="34">
+        <v>42986</v>
+      </c>
+      <c r="F92" s="34">
+        <v>42986</v>
+      </c>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
     </row>
     <row r="93" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="22" t="s">
+      <c r="A93" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C93" s="20">
+      <c r="C93" s="16">
         <v>1</v>
       </c>
-      <c r="D93" s="19" t="s">
+      <c r="D93" s="15" t="s">
         <v>89</v>
       </c>
       <c r="E93" s="4"/>
@@ -4808,21 +5229,36 @@
       <c r="I93" s="7"/>
     </row>
     <row r="94" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="7"/>
+      <c r="A94" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94" s="16">
+        <v>1</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E94" s="34">
+        <v>42986</v>
+      </c>
+      <c r="F94" s="34">
+        <v>42986</v>
+      </c>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
     </row>
     <row r="95" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
+      <c r="B95" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95" s="36">
+        <v>1</v>
+      </c>
+      <c r="D95" s="16"/>
       <c r="E95" s="4"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
@@ -4830,10 +5266,13 @@
       <c r="I95" s="7"/>
     </row>
     <row r="96" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
+      <c r="B96" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C96" s="36">
+        <v>1</v>
+      </c>
+      <c r="D96" s="16"/>
       <c r="E96" s="4"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
@@ -4841,10 +5280,13 @@
       <c r="I96" s="7"/>
     </row>
     <row r="97" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
+      <c r="B97" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C97" s="36">
+        <v>1</v>
+      </c>
+      <c r="D97" s="16"/>
       <c r="E97" s="4"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
@@ -4852,10 +5294,13 @@
       <c r="I97" s="7"/>
     </row>
     <row r="98" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="21"/>
+      <c r="B98" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C98" s="37">
+        <v>1</v>
+      </c>
+      <c r="D98" s="17"/>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
@@ -4863,18 +5308,152 @@
       <c r="I98" s="7"/>
     </row>
     <row r="99" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
+      <c r="B99" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C99" s="37">
+        <v>1</v>
+      </c>
+      <c r="D99" s="17"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
     </row>
+    <row r="100" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C100" s="37">
+        <v>1</v>
+      </c>
+      <c r="D100" s="17"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
+    </row>
+    <row r="101" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+    </row>
+    <row r="102" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="119">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C59:C60"/>
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="D15:D16"/>
@@ -4899,101 +5478,6 @@
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D65:D66"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://www.arduinoall.com/product/16"/>
@@ -5035,7 +5519,7 @@
     <hyperlink ref="B84" r:id="rId37" display="https://www.arduinoall.com/product/1698"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId38"/>
   <drawing r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>